<commit_message>
Updated CSE Needfinding Project
</commit_message>
<xml_diff>
--- a/docs/CSE Project/Diary Study/Diary Study Form (Responses).xlsx
+++ b/docs/CSE Project/Diary Study/Diary Study Form (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="142">
   <si>
     <t>Timestamp</t>
   </si>
@@ -60,6 +60,384 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>straussj9926@my.sduhsd.net</t>
+  </si>
+  <si>
+    <t>GMail, Discord, INstagram.</t>
+  </si>
+  <si>
+    <t>I just looked at stuff not much</t>
+  </si>
+  <si>
+    <t>No problems</t>
+  </si>
+  <si>
+    <t>gokhalen9693@my.sduhsd.net</t>
+  </si>
+  <si>
+    <t>Day 2</t>
+  </si>
+  <si>
+    <t>iMessage and email because they’re the most commonly used among my friends and teachers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texting friends and emailing teachers </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C’est juste que l’iMessage est mis à jour et ça c’est différent qu’avant donc peut être ils doivent créer un documentaire qui explique les changements </t>
+  </si>
+  <si>
+    <t>ambrosem381@carlsbadusd.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiktok instagram imessage snapchat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">taking to friends find out information </t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>goldsmithz1481@my.sduhsd.net</t>
+  </si>
+  <si>
+    <t>Imessage because its easiest</t>
+  </si>
+  <si>
+    <t>Texting friends</t>
+  </si>
+  <si>
+    <t>People dont see my message right away</t>
+  </si>
+  <si>
+    <t>Gmail</t>
+  </si>
+  <si>
+    <t>For keeping track of schoolwork and communicating with friends</t>
+  </si>
+  <si>
+    <t>paula.rodriguezpaniagua.08@gmail.com</t>
+  </si>
+  <si>
+    <t>Instagram, TikTok, Snapchat</t>
+  </si>
+  <si>
+    <t>Talking to friends, being entertained</t>
+  </si>
+  <si>
+    <t>Nope</t>
+  </si>
+  <si>
+    <t>Day 3</t>
+  </si>
+  <si>
+    <t>iMessage, email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talking to friends, emailing teachers and counselors </t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Yes. I used iMessage</t>
+  </si>
+  <si>
+    <t>Imessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texting my friends </t>
+  </si>
+  <si>
+    <t>Not fast enough responses</t>
+  </si>
+  <si>
+    <t>Gmail since it is the only one I have</t>
+  </si>
+  <si>
+    <t>I mainly just used it to keep track of assignments</t>
+  </si>
+  <si>
+    <t>I didn't need to communicate with peers over the course of the diary study.</t>
+  </si>
+  <si>
+    <t>snapchat instagram tiktok messages gmail</t>
+  </si>
+  <si>
+    <t>talking to friends finding our information and helping with homework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my snapchat ai wouldn’t answer my question </t>
+  </si>
+  <si>
+    <t>yessengeldyd8038@my.sduhsd.net</t>
+  </si>
+  <si>
+    <t>Nothing in particular</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>mozaffara1424@my.sduhsd.net</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>I talked with my friends about a class</t>
+  </si>
+  <si>
+    <t>paik2119@my.sduhsd.net</t>
+  </si>
+  <si>
+    <t>Need to use it for classified reasons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gmail, Instagram, Discord, yes i used them becuase they are populaire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding out information. </t>
+  </si>
+  <si>
+    <t>I had no problems</t>
+  </si>
+  <si>
+    <t>szyukiwu@gmail.com</t>
+  </si>
+  <si>
+    <t>Talking to friends</t>
+  </si>
+  <si>
+    <t>Snapchat, to text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talking to friends </t>
+  </si>
+  <si>
+    <t>My chats disappear after a period of time which is annoying</t>
+  </si>
+  <si>
+    <t>I did need to communicate with peers, specifically about math, but there wasnt a super efficient way to communicate in a timely manner. I used imessage and snapchat, but i wish there was another app that i could use in order to get in contact with maybe a peer tutor online</t>
+  </si>
+  <si>
+    <t>rodriguezpaniap7968@my.sduhsd.net</t>
+  </si>
+  <si>
+    <t>Instagram TikTok Snapchat, so I can talk to my friends in a quick and convenient way</t>
+  </si>
+  <si>
+    <t>zengv9840@my.sduhsd.net</t>
+  </si>
+  <si>
+    <t>snap</t>
+  </si>
+  <si>
+    <t>friends</t>
+  </si>
+  <si>
+    <t>huanga0189@my.sudhsd.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gmail and Discord </t>
+  </si>
+  <si>
+    <t>to text my friends and email classmates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All of the above </t>
+  </si>
+  <si>
+    <t>Finding info</t>
+  </si>
+  <si>
+    <t>Yes I used messages and discord</t>
+  </si>
+  <si>
+    <t>snapchat tiktok insta messages gmail</t>
+  </si>
+  <si>
+    <t>talking to friends and finding info</t>
+  </si>
+  <si>
+    <t>nah</t>
+  </si>
+  <si>
+    <t>yes on snap</t>
+  </si>
+  <si>
+    <t>snap and insta</t>
+  </si>
+  <si>
+    <t>talking to friends</t>
+  </si>
+  <si>
+    <t>gmail and instagram</t>
+  </si>
+  <si>
+    <t>I texted my friends and also emailed a classmate about a group project</t>
+  </si>
+  <si>
+    <t>It was kinda annoying to email my classmate back and forth and he didn't have instagram</t>
+  </si>
+  <si>
+    <t>Sapchat Instagram to talk to my friends</t>
+  </si>
+  <si>
+    <t>Yes but I couldn't so I just talked to them during school</t>
+  </si>
+  <si>
+    <t>Instagram, snapchat</t>
+  </si>
+  <si>
+    <t>Talking to my team</t>
+  </si>
+  <si>
+    <t>couldnt load properly</t>
+  </si>
+  <si>
+    <t>guob4389@my.sduhsd.net</t>
+  </si>
+  <si>
+    <t>Discord</t>
+  </si>
+  <si>
+    <t>Gmail, Chat</t>
+  </si>
+  <si>
+    <t>Talking to my teacher</t>
+  </si>
+  <si>
+    <t>Format was weird</t>
+  </si>
+  <si>
+    <t>Discord and Gmail</t>
+  </si>
+  <si>
+    <t>I texted my friends on discord and emailed my teacher on gmail</t>
+  </si>
+  <si>
+    <t>gmail and insta</t>
+  </si>
+  <si>
+    <t>friends and a teacher</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no</t>
+  </si>
+  <si>
+    <t>not peers but had to message my teacher for an assignment</t>
+  </si>
+  <si>
+    <t>discord</t>
+  </si>
+  <si>
+    <t>messaged my friends</t>
+  </si>
+  <si>
+    <t>Yes. I needed to contact my classmates for a group project and I also had to email my teacher about an assignment</t>
+  </si>
+  <si>
+    <t>discord, instagram</t>
+  </si>
+  <si>
+    <t>sending message to my club</t>
+  </si>
+  <si>
+    <t>discord gmail</t>
+  </si>
+  <si>
+    <t>talking to friends, group project for club</t>
+  </si>
+  <si>
+    <t>Yes. I used Discord to contact them.</t>
+  </si>
+  <si>
+    <t>Gmail, Discord, instagram</t>
+  </si>
+  <si>
+    <t>nope</t>
+  </si>
+  <si>
+    <t>Gmail, imessage, discord, instagram</t>
+  </si>
+  <si>
+    <t>Talking to friends, finding information</t>
+  </si>
+  <si>
+    <t>Yes, most of the time I can successfully contact them. I used discord and imessage</t>
+  </si>
+  <si>
+    <t>iMessage, Discord, Instagram</t>
+  </si>
+  <si>
+    <t>Talking to freinds</t>
+  </si>
+  <si>
+    <t>Couldnt kick someone</t>
+  </si>
+  <si>
+    <t>Yeah, I used iMessage.</t>
+  </si>
+  <si>
+    <t>Gmail, Discord</t>
+  </si>
+  <si>
+    <t>Needed to talk to my partner</t>
+  </si>
+  <si>
+    <t>Couldnt find my partner innitially</t>
+  </si>
+  <si>
+    <t>I was able to use discord to talk to my partner.</t>
+  </si>
+  <si>
+    <t>iMessage, Instagram</t>
+  </si>
+  <si>
+    <t>I texted my family on imessage and friends on insta</t>
+  </si>
+  <si>
+    <t>I had to message a classmate for a project and it was really annoying to do on gmail</t>
+  </si>
+  <si>
+    <t>dr.hungry886@gmail.com</t>
+  </si>
+  <si>
+    <t>Gmail, iMessage, Discord</t>
+  </si>
+  <si>
+    <t>talking to friends, finding out information</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>No not really, if I must i usually use discord and pin them a lot of times</t>
+  </si>
+  <si>
+    <t>wuy9816@my.sduhsd.net</t>
+  </si>
+  <si>
+    <t>not really</t>
+  </si>
+  <si>
+    <t>Gmail, iMessage, Discord, Instagram</t>
+  </si>
+  <si>
+    <t>i dont have any</t>
+  </si>
+  <si>
+    <t>talking to friends, finding out information, working on group projects</t>
+  </si>
+  <si>
+    <t>not at all</t>
+  </si>
+  <si>
+    <t>Yes, when that happens I just call them if I have their number. If not I just go to google classroom and find their email.</t>
   </si>
 </sst>
 </file>
@@ -69,7 +447,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -81,16 +459,40 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor rgb="FFF8F9FA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border/>
     <border>
       <left style="thin">
@@ -187,7 +589,7 @@
         <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF442F65"/>
+        <color rgb="FFF8F9FA"/>
       </bottom>
     </border>
     <border>
@@ -201,6 +603,62 @@
         <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
     </border>
@@ -208,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -236,6 +694,97 @@
     <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -279,11 +828,15 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="1">
+  <tableStyles count="2">
     <tableStyle count="3" pivot="0" name="Form Responses 1-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Form Responses 1-style 2">
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -294,7 +847,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G3" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G46" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="7">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -305,6 +858,21 @@
     <tableColumn name="ONLY complete this question on DAY 3_x000a__x000a_During the days you completed this diary study, did you ever need to communicate with peers for school-related purposes for any reason? Were you able to successfully contact them? If so, which communication app(s) did you use to communicate with them?" id="7"/>
   </tableColumns>
   <tableStyleInfo name="Form Responses 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A47:G48" displayName="Table_1" name="Table_1" id="2">
+  <tableColumns count="7">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+  </tableColumns>
+  <tableStyleInfo name="Form Responses 1-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -585,10 +1153,937 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="9">
+        <v>45723.56024196759</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7">
+        <v>45723.66309103009</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9">
+        <v>45726.39274553241</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7">
+        <v>45726.39967108796</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="9">
+        <v>45726.42647815972</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7">
+        <v>45726.49273068287</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="9">
+        <v>45727.35983238426</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7">
+        <v>45727.416637013885</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="9">
+        <v>45727.421226516206</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7">
+        <v>45727.68021390046</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="9">
+        <v>45727.7812962963</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7">
+        <v>45728.13431712963</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="9">
+        <v>45728.294756944444</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7">
+        <v>45728.36181883102</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9">
+        <v>45728.38483119213</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7">
+        <v>45728.39051783565</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="9">
+        <v>45728.48679859954</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="7">
+        <v>45728.50231481482</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="14">
+        <v>45728.535891203705</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="7">
+        <v>45728.59025462963</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="9">
+        <v>45728.89427329861</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9">
+        <v>45729.04351851852</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="9">
+        <v>45729.11896990741</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="19">
+        <v>45729.35832175926</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="7">
+        <v>45729.40677083333</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="24">
+        <v>45729.473599537036</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="9">
+        <v>45729.50603009259</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="25">
+        <v>45729.697384259256</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="27"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="9">
+        <v>45730.100173611114</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7">
+        <v>45730.371757650464</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="29">
+        <v>45730.37217238426</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="31"/>
+      <c r="G34" s="32"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="33">
+        <v>45730.372555208334</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="9">
+        <v>45730.37339288194</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="7">
+        <v>45730.37395417824</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="9">
+        <v>45730.378969907404</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="7">
+        <v>45730.381394745375</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="9">
+        <v>45730.39048611111</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="7">
+        <v>45730.38940364584</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="9">
+        <v>45730.38955978009</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="7">
+        <v>45730.38993822917</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="9">
+        <v>45730.39061582176</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="7">
+        <v>45730.3908015162</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="35">
+        <v>45730.391353125</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E46" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="F46" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="38"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>